<commit_message>
vault backup: 2025-11-19 16:08:09
</commit_message>
<xml_diff>
--- a/00_Inbox/Beraring Temp monitoring capital estimate.xlsx
+++ b/00_Inbox/Beraring Temp monitoring capital estimate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10064957\My Drive\GDVault\MarthaVault\00_Inbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DA6047C-6DA7-49B5-A832-61CD01D0D412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4944EDDD-4873-406D-8D59-F12E915546CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{26256806-646B-410B-99AC-2ABEBF893D43}"/>
   </bookViews>
@@ -66,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{0E8AF660-02A3-469D-B53C-48123CE14D66}">
+    <comment ref="H28" authorId="0" shapeId="0" xr:uid="{0E8AF660-02A3-469D-B53C-48123CE14D66}">
       <text>
         <r>
           <rPr>
@@ -90,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{34497327-8759-4969-9E67-8203E18104A7}">
+    <comment ref="H36" authorId="0" shapeId="0" xr:uid="{34497327-8759-4969-9E67-8203E18104A7}">
       <text>
         <r>
           <rPr>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
   <si>
     <t>Glue</t>
   </si>
@@ -296,6 +296,54 @@
   </si>
   <si>
     <t>N3 Current</t>
+  </si>
+  <si>
+    <t>NR1 conveyor</t>
+  </si>
+  <si>
+    <t>NR2 conveyor</t>
+  </si>
+  <si>
+    <t>NR3 conveyor</t>
+  </si>
+  <si>
+    <t>NR4 conveyor</t>
+  </si>
+  <si>
+    <t>NR5 conveyor</t>
+  </si>
+  <si>
+    <t>NR6 conveyor</t>
+  </si>
+  <si>
+    <t>NR7 conveyor</t>
+  </si>
+  <si>
+    <t>NR8 conveyor</t>
+  </si>
+  <si>
+    <t>NR9 conveyor</t>
+  </si>
+  <si>
+    <t>NR10 conveyor</t>
+  </si>
+  <si>
+    <t>NR11 conveyor</t>
+  </si>
+  <si>
+    <t>ST07 conveyor</t>
+  </si>
+  <si>
+    <t>US 01 conveyor</t>
+  </si>
+  <si>
+    <t>US 02 conveyor</t>
+  </si>
+  <si>
+    <t>LS01 conveyor</t>
+  </si>
+  <si>
+    <t>LS02 conveyor</t>
   </si>
 </sst>
 </file>
@@ -303,7 +351,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="_-[$R-1C09]* #,##0_-;\-[$R-1C09]* #,##0_-;_-[$R-1C09]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$R-1C09]* #,##0_-;\-[$R-1C09]* #,##0_-;_-[$R-1C09]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -383,12 +431,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -983,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978F4542-314C-4B68-BEB6-A1F300014BA4}">
-  <dimension ref="B1:P36"/>
+  <dimension ref="B1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,102 +1182,432 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="5">
-        <f>SUM(P2:P3)</f>
-        <v>468430</v>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4">
+        <f>+G4/2</f>
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <f>+G4*Sheet1!$E$2</f>
+        <v>30108</v>
+      </c>
+      <c r="J4" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G4</f>
+        <v>1660</v>
+      </c>
+      <c r="K4" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G4</f>
+        <v>2281</v>
+      </c>
+      <c r="L4" s="4">
+        <f>+Sheet1!$E$4*H4</f>
+        <v>20480</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4" s="4">
+        <f>+M4*Sheet1!$C$13</f>
+        <v>53200</v>
+      </c>
+      <c r="O4" s="4">
+        <f>+M4*Sheet1!$C$12</f>
+        <v>8800</v>
+      </c>
+      <c r="P4" s="4">
+        <f t="shared" ref="P4:P19" si="0">+N4+L4+K4+J4+I4</f>
+        <v>107729</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="6"/>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F19" si="1">+G5/2</f>
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <f>+G5*Sheet1!$E$2</f>
+        <v>105378</v>
+      </c>
+      <c r="J5" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G5</f>
+        <v>5810</v>
+      </c>
+      <c r="K5" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G5</f>
+        <v>7983.5</v>
+      </c>
+      <c r="L5" s="4">
+        <f>+Sheet1!$E$4*H5</f>
+        <v>20480</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+      <c r="N5" s="4">
+        <f>+M5*Sheet1!$C$13</f>
+        <v>66500</v>
+      </c>
+      <c r="O5" s="4">
+        <f>+M5*Sheet1!$C$12</f>
+        <v>11000</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" si="0"/>
+        <v>206151.5</v>
+      </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N6" t="s">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>24</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6" s="4">
+        <f>+G6*Sheet1!$E$2</f>
+        <v>180648</v>
+      </c>
+      <c r="J6" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G6</f>
+        <v>9960</v>
+      </c>
+      <c r="K6" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G6</f>
+        <v>13686</v>
+      </c>
+      <c r="L6" s="4">
+        <f>+Sheet1!$E$4*H6</f>
+        <v>40960</v>
+      </c>
+      <c r="M6">
+        <v>6</v>
+      </c>
+      <c r="N6" s="4">
+        <f>+M6*Sheet1!$C$13</f>
+        <v>79800</v>
+      </c>
+      <c r="O6" s="4">
+        <f>+M6*Sheet1!$C$12</f>
+        <v>13200</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="0"/>
+        <v>325054</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="P6">
-        <f>+Sheet1!$C$11</f>
-        <v>16512</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N7" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7">
-        <f>+Sheet1!$C$10</f>
-        <v>9600</v>
+      <c r="G7">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
+        <f>+G7*Sheet1!$E$2</f>
+        <v>105378</v>
+      </c>
+      <c r="J7" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G7</f>
+        <v>5810</v>
+      </c>
+      <c r="K7" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G7</f>
+        <v>7983.5</v>
+      </c>
+      <c r="L7" s="4">
+        <f>+Sheet1!$E$4*H7</f>
+        <v>20480</v>
+      </c>
+      <c r="M7">
+        <v>7</v>
+      </c>
+      <c r="N7" s="4">
+        <f>+M7*Sheet1!$C$13</f>
+        <v>93100</v>
+      </c>
+      <c r="O7" s="4">
+        <f>+M7*Sheet1!$C$12</f>
+        <v>15400</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="0"/>
+        <v>232751.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>14</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <f>+G8*Sheet1!$E$2</f>
+        <v>105378</v>
+      </c>
+      <c r="J8" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G8</f>
+        <v>5810</v>
+      </c>
+      <c r="K8" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G8</f>
+        <v>7983.5</v>
+      </c>
+      <c r="L8" s="4">
+        <f>+Sheet1!$E$4*H8</f>
+        <v>20480</v>
+      </c>
+      <c r="M8">
+        <v>8</v>
+      </c>
+      <c r="N8" s="4">
+        <f>+M8*Sheet1!$C$13</f>
+        <v>106400</v>
+      </c>
+      <c r="O8" s="4">
+        <f>+M8*Sheet1!$C$12</f>
+        <v>17600</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="0"/>
+        <v>246051.5</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="M9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9">
-        <f>+P4+P6+P7</f>
-        <v>494542</v>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
+        <f>+G9*Sheet1!$E$2</f>
+        <v>105378</v>
+      </c>
+      <c r="J9" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G9</f>
+        <v>5810</v>
+      </c>
+      <c r="K9" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G9</f>
+        <v>7983.5</v>
+      </c>
+      <c r="L9" s="4">
+        <f>+Sheet1!$E$4*H9</f>
+        <v>20480</v>
+      </c>
+      <c r="M9">
+        <v>9</v>
+      </c>
+      <c r="N9" s="4">
+        <f>+M9*Sheet1!$C$13</f>
+        <v>119700</v>
+      </c>
+      <c r="O9" s="4">
+        <f>+M9*Sheet1!$C$12</f>
+        <v>19800</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="0"/>
+        <v>259351.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
+        <f>+G10*Sheet1!$E$2</f>
+        <v>105378</v>
+      </c>
+      <c r="J10" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G10</f>
+        <v>5810</v>
+      </c>
+      <c r="K10" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G10</f>
+        <v>7983.5</v>
+      </c>
+      <c r="L10" s="4">
+        <f>+Sheet1!$E$4*H10</f>
+        <v>20480</v>
+      </c>
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="N10" s="4">
+        <f>+M10*Sheet1!$C$13</f>
+        <v>133000</v>
+      </c>
+      <c r="O10" s="4">
+        <f>+M10*Sheet1!$C$12</f>
+        <v>22000</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="0"/>
+        <v>272651.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
+        <f>+G11*Sheet1!$E$2</f>
+        <v>105378</v>
+      </c>
+      <c r="J11" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G11</f>
+        <v>5810</v>
+      </c>
+      <c r="K11" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G11</f>
+        <v>7983.5</v>
+      </c>
+      <c r="L11" s="4">
+        <f>+Sheet1!$E$4*H11</f>
+        <v>20480</v>
+      </c>
+      <c r="M11">
+        <v>11</v>
+      </c>
+      <c r="N11" s="4">
+        <f>+M11*Sheet1!$C$13</f>
+        <v>146300</v>
+      </c>
+      <c r="O11" s="4">
+        <f>+M11*Sheet1!$C$12</f>
+        <v>24200</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" si="0"/>
+        <v>285951.5</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>53</v>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <f>+G12*Sheet1!$E$2</f>
+        <v>30108</v>
+      </c>
+      <c r="J12" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G12</f>
+        <v>1660</v>
+      </c>
+      <c r="K12" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G12</f>
+        <v>2281</v>
+      </c>
+      <c r="L12" s="4">
+        <f>+Sheet1!$E$4*H12</f>
+        <v>20480</v>
+      </c>
+      <c r="M12">
+        <v>12</v>
+      </c>
+      <c r="N12" s="4">
+        <f>+M12*Sheet1!$C$13</f>
+        <v>159600</v>
+      </c>
+      <c r="O12" s="4">
+        <f>+M12*Sheet1!$C$12</f>
+        <v>26400</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="0"/>
+        <v>214129</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F13">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="G13">
         <v>14</v>
       </c>
       <c r="H13">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I13" s="4">
         <f>+G13*Sheet1!$E$2</f>
@@ -1245,336 +1623,757 @@
       </c>
       <c r="L13" s="4">
         <f>+Sheet1!$E$4*H13</f>
-        <v>143360</v>
+        <v>20480</v>
       </c>
       <c r="M13">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="N13" s="4">
         <f>+M13*Sheet1!$C$13</f>
-        <v>93100</v>
+        <v>172900</v>
       </c>
       <c r="O13" s="4">
         <f>+M13*Sheet1!$C$12</f>
+        <v>28600</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="0"/>
+        <v>312551.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>18</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <f>+G14*Sheet1!$E$2</f>
+        <v>135486</v>
+      </c>
+      <c r="J14" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G14</f>
+        <v>7470</v>
+      </c>
+      <c r="K14" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G14</f>
+        <v>10264.5</v>
+      </c>
+      <c r="L14" s="4">
+        <f>+Sheet1!$E$4*H14</f>
+        <v>20480</v>
+      </c>
+      <c r="M14">
+        <v>14</v>
+      </c>
+      <c r="N14" s="4">
+        <f>+M14*Sheet1!$C$13</f>
+        <v>186200</v>
+      </c>
+      <c r="O14" s="4">
+        <f>+M14*Sheet1!$C$12</f>
+        <v>30800</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="0"/>
+        <v>359900.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>16</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <f>+G15*Sheet1!$E$2</f>
+        <v>120432</v>
+      </c>
+      <c r="J15" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G15</f>
+        <v>6640</v>
+      </c>
+      <c r="K15" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G15</f>
+        <v>9124</v>
+      </c>
+      <c r="L15" s="4">
+        <f>+Sheet1!$E$4*H15</f>
+        <v>20480</v>
+      </c>
+      <c r="M15">
+        <v>15</v>
+      </c>
+      <c r="N15" s="4">
+        <f>+M15*Sheet1!$C$13</f>
+        <v>199500</v>
+      </c>
+      <c r="O15" s="4">
+        <f>+M15*Sheet1!$C$12</f>
+        <v>33000</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" si="0"/>
+        <v>356176</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>18</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
+        <f>+G16*Sheet1!$E$2</f>
+        <v>135486</v>
+      </c>
+      <c r="J16" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G16</f>
+        <v>7470</v>
+      </c>
+      <c r="K16" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G16</f>
+        <v>10264.5</v>
+      </c>
+      <c r="L16" s="4">
+        <f>+Sheet1!$E$4*H16</f>
+        <v>20480</v>
+      </c>
+      <c r="M16">
+        <v>16</v>
+      </c>
+      <c r="N16" s="4">
+        <f>+M16*Sheet1!$C$13</f>
+        <v>212800</v>
+      </c>
+      <c r="O16" s="4">
+        <f>+M16*Sheet1!$C$12</f>
+        <v>35200</v>
+      </c>
+      <c r="P16" s="4">
+        <f t="shared" si="0"/>
+        <v>386500.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4">
+        <f>+G17*Sheet1!$E$2</f>
+        <v>120432</v>
+      </c>
+      <c r="J17" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G17</f>
+        <v>6640</v>
+      </c>
+      <c r="K17" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G17</f>
+        <v>9124</v>
+      </c>
+      <c r="L17" s="4">
+        <f>+Sheet1!$E$4*H17</f>
+        <v>20480</v>
+      </c>
+      <c r="M17">
+        <v>17</v>
+      </c>
+      <c r="N17" s="4">
+        <f>+M17*Sheet1!$C$13</f>
+        <v>226100</v>
+      </c>
+      <c r="O17" s="4">
+        <f>+M17*Sheet1!$C$12</f>
+        <v>37400</v>
+      </c>
+      <c r="P17" s="4">
+        <f t="shared" si="0"/>
+        <v>382776</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>14</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4">
+        <f>+G18*Sheet1!$E$2</f>
+        <v>105378</v>
+      </c>
+      <c r="J18" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G18</f>
+        <v>5810</v>
+      </c>
+      <c r="K18" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G18</f>
+        <v>7983.5</v>
+      </c>
+      <c r="L18" s="4">
+        <f>+Sheet1!$E$4*H18</f>
+        <v>20480</v>
+      </c>
+      <c r="M18">
+        <v>18</v>
+      </c>
+      <c r="N18" s="4">
+        <f>+M18*Sheet1!$C$13</f>
+        <v>239400</v>
+      </c>
+      <c r="O18" s="4">
+        <f>+M18*Sheet1!$C$12</f>
+        <v>39600</v>
+      </c>
+      <c r="P18" s="4">
+        <f t="shared" si="0"/>
+        <v>379051.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G19">
+        <v>14</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" s="4">
+        <f>+G19*Sheet1!$E$2</f>
+        <v>105378</v>
+      </c>
+      <c r="J19" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G19</f>
+        <v>5810</v>
+      </c>
+      <c r="K19" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G19</f>
+        <v>7983.5</v>
+      </c>
+      <c r="L19" s="4">
+        <f>+Sheet1!$E$4*H19</f>
+        <v>20480</v>
+      </c>
+      <c r="M19">
+        <v>19</v>
+      </c>
+      <c r="N19" s="4">
+        <f>+M19*Sheet1!$C$13</f>
+        <v>252700</v>
+      </c>
+      <c r="O19" s="4">
+        <f>+M19*Sheet1!$C$12</f>
+        <v>41800</v>
+      </c>
+      <c r="P19" s="4">
+        <f t="shared" si="0"/>
+        <v>392351.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="5">
+        <f>SUM(P2:P19)</f>
+        <v>5187558.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>7</v>
+      </c>
+      <c r="P22" s="4">
+        <f>+Sheet1!$C$11*4</f>
+        <v>66048</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>43</v>
+      </c>
+      <c r="P23" s="4">
+        <f>+Sheet1!$C$10*4</f>
+        <v>38400</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M25" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="O25" s="8"/>
+      <c r="P25" s="9">
+        <f>+P20+P22+P23</f>
+        <v>5292006.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29">
+        <v>7</v>
+      </c>
+      <c r="G29">
+        <v>14</v>
+      </c>
+      <c r="H29">
+        <v>7</v>
+      </c>
+      <c r="I29" s="4">
+        <f>+G29*Sheet1!$E$2</f>
+        <v>105378</v>
+      </c>
+      <c r="J29" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G29</f>
+        <v>5810</v>
+      </c>
+      <c r="K29" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G29</f>
+        <v>7983.5</v>
+      </c>
+      <c r="L29" s="4">
+        <f>+Sheet1!$E$4*H29</f>
+        <v>143360</v>
+      </c>
+      <c r="M29">
+        <v>7</v>
+      </c>
+      <c r="N29" s="4">
+        <f>+M29*Sheet1!$C$13</f>
+        <v>93100</v>
+      </c>
+      <c r="O29" s="4">
+        <f>+M29*Sheet1!$C$12</f>
         <v>15400</v>
       </c>
-      <c r="P13" s="4">
-        <f>+N13+L13+K13+J13+I13</f>
+      <c r="P29" s="4">
+        <f>+N29+L29+K29+J29+I29</f>
         <v>355631.5</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N14" s="6" t="s">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="O14" s="6"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N15" t="s">
+      <c r="O30" s="6"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
         <v>7</v>
       </c>
-      <c r="P15">
+      <c r="P31" s="4">
         <f>+Sheet1!$C$11</f>
         <v>16512</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N16" t="s">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
         <v>43</v>
       </c>
-      <c r="P16">
+      <c r="P32" s="4">
         <f>+Sheet1!$C$10</f>
         <v>9600</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="M17" s="10" t="s">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M33" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="N17" s="7" t="s">
+      <c r="N33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="O17" s="8"/>
-      <c r="P17" s="9">
-        <f>+P16+P15+P13</f>
+      <c r="O33" s="8"/>
+      <c r="P33" s="9">
+        <f>+P32+P31+P29</f>
         <v>381743.5</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J36" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="L36" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M36" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N20" s="2" t="s">
+      <c r="N36" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="O20" s="2" t="s">
+      <c r="O36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P20" s="2" t="s">
+      <c r="P36" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F21">
+      <c r="F37">
         <v>8</v>
       </c>
-      <c r="G21">
+      <c r="G37">
         <v>16</v>
       </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21" s="4">
-        <f>+G21*Sheet1!$E$2</f>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37" s="4">
+        <f>+G37*Sheet1!$E$2</f>
         <v>120432</v>
       </c>
-      <c r="J21" s="4">
-        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G21</f>
+      <c r="J37" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G37</f>
         <v>6640</v>
       </c>
-      <c r="K21" s="4">
-        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G21</f>
+      <c r="K37" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G37</f>
         <v>9124</v>
       </c>
-      <c r="L21" s="4">
-        <f>+Sheet1!$E$4*H21</f>
+      <c r="L37" s="4">
+        <f>+Sheet1!$E$4*H37</f>
         <v>20480</v>
       </c>
-      <c r="M21">
+      <c r="M37">
         <v>7</v>
       </c>
-      <c r="N21" s="4">
-        <f>+M21*Sheet1!$C$13</f>
+      <c r="N37" s="4">
+        <f>+M37*Sheet1!$C$13</f>
         <v>93100</v>
       </c>
-      <c r="O21" s="4">
-        <f>+M21*Sheet1!$C$12</f>
+      <c r="O37" s="4">
+        <f>+M37*Sheet1!$C$12</f>
         <v>15400</v>
       </c>
-      <c r="P21" s="4">
-        <f>+N21+L21+K21+J21+I21</f>
+      <c r="P37" s="4">
+        <f>+N37+L37+K37+J37+I37</f>
         <v>249776</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F22">
+      <c r="F38">
         <v>9</v>
       </c>
-      <c r="G22">
+      <c r="G38">
         <v>18</v>
       </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22" s="4">
-        <f>+G22*Sheet1!$E$2</f>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38" s="4">
+        <f>+G38*Sheet1!$E$2</f>
         <v>135486</v>
       </c>
-      <c r="J22" s="4">
-        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G22</f>
+      <c r="J38" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G38</f>
         <v>7470</v>
       </c>
-      <c r="K22" s="4">
-        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G22</f>
+      <c r="K38" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G38</f>
         <v>10264.5</v>
       </c>
-      <c r="L22" s="4">
-        <f>+Sheet1!$E$4*H22</f>
+      <c r="L38" s="4">
+        <f>+Sheet1!$E$4*H38</f>
         <v>20480</v>
       </c>
-      <c r="M22">
+      <c r="M38">
         <v>7</v>
       </c>
-      <c r="N22" s="4">
-        <f>+M22*Sheet1!$C$13</f>
+      <c r="N38" s="4">
+        <f>+M38*Sheet1!$C$13</f>
         <v>93100</v>
       </c>
-      <c r="O22" s="4">
-        <f>+M22*Sheet1!$C$12</f>
+      <c r="O38" s="4">
+        <f>+M38*Sheet1!$C$12</f>
         <v>15400</v>
       </c>
-      <c r="P22" s="4">
-        <f>+N22+L22+K22+J22+I22</f>
+      <c r="P38" s="4">
+        <f>+N38+L38+K38+J38+I38</f>
         <v>266800.5</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F23">
+      <c r="F39">
         <v>8</v>
       </c>
-      <c r="G23">
+      <c r="G39">
         <v>16</v>
       </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23" s="4">
-        <f>+G23*Sheet1!$E$2</f>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39" s="4">
+        <f>+G39*Sheet1!$E$2</f>
         <v>120432</v>
       </c>
-      <c r="J23" s="4">
-        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G23</f>
+      <c r="J39" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G39</f>
         <v>6640</v>
       </c>
-      <c r="K23" s="4">
-        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G23</f>
+      <c r="K39" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G39</f>
         <v>9124</v>
       </c>
-      <c r="L23" s="4">
-        <f>+Sheet1!$E$4*H23</f>
+      <c r="L39" s="4">
+        <f>+Sheet1!$E$4*H39</f>
         <v>20480</v>
       </c>
-      <c r="M23">
+      <c r="M39">
         <v>7</v>
       </c>
-      <c r="N23" s="4">
-        <f>+M23*Sheet1!$C$13</f>
+      <c r="N39" s="4">
+        <f>+M39*Sheet1!$C$13</f>
         <v>93100</v>
       </c>
-      <c r="O23" s="4">
-        <f>+M23*Sheet1!$C$12</f>
+      <c r="O39" s="4">
+        <f>+M39*Sheet1!$C$12</f>
         <v>15400</v>
       </c>
-      <c r="P23" s="4">
-        <f t="shared" ref="P23:P24" si="0">+N23+L23+K23+J23+I23</f>
+      <c r="P39" s="4">
+        <f t="shared" ref="P39:P40" si="2">+N39+L39+K39+J39+I39</f>
         <v>249776</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
         <v>2</v>
       </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24" s="4">
-        <f>+G24*Sheet1!$E$2</f>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40" s="4">
+        <f>+G40*Sheet1!$E$2</f>
         <v>15054</v>
       </c>
-      <c r="J24" s="4">
-        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G24</f>
+      <c r="J40" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G40</f>
         <v>830</v>
       </c>
-      <c r="K24" s="4">
-        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G24</f>
+      <c r="K40" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G40</f>
         <v>1140.5</v>
       </c>
-      <c r="L24" s="4">
-        <f>+Sheet1!$E$4*H24</f>
+      <c r="L40" s="4">
+        <f>+Sheet1!$E$4*H40</f>
         <v>20480</v>
       </c>
-      <c r="M24">
+      <c r="M40">
         <v>7</v>
       </c>
-      <c r="N24" s="4">
-        <f>+M24*Sheet1!$C$13</f>
+      <c r="N40" s="4">
+        <f>+M40*Sheet1!$C$13</f>
         <v>93100</v>
       </c>
-      <c r="O24" s="4">
-        <f>+M24*Sheet1!$C$12</f>
+      <c r="O40" s="4">
+        <f>+M40*Sheet1!$C$12</f>
         <v>15400</v>
       </c>
-      <c r="P24" s="4">
-        <f t="shared" si="0"/>
+      <c r="P40" s="4">
+        <f t="shared" si="2"/>
         <v>130604.5</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N25" s="6" t="s">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="N41" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="O41" s="4"/>
+      <c r="P41" s="5">
+        <f>SUM(P37:P40)</f>
+        <v>896957</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N42" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="O25" s="6"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N26" t="s">
+      <c r="O42" s="6"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
         <v>7</v>
       </c>
-      <c r="P26">
-        <f>+Sheet1!$C$11</f>
-        <v>16512</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N27" t="s">
+      <c r="P43" s="4">
+        <f>+Sheet1!$C$11*2</f>
+        <v>33024</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
         <v>43</v>
       </c>
-      <c r="P27">
-        <f>+Sheet1!$C$10</f>
-        <v>9600</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="M28" s="10" t="s">
+      <c r="P44" s="4">
+        <f>+Sheet1!$C$10*2</f>
+        <v>19200</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M45" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="N28" s="7" t="s">
+      <c r="N45" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="O28" s="8"/>
-      <c r="P28" s="9">
-        <f>+P27+P26+P24+P21+P22+P23</f>
-        <v>923069</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
+      <c r="O45" s="8"/>
+      <c r="P45" s="9">
+        <f>+P44+P43+P40+P37+P38+P39</f>
+        <v>949181</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>23</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C51" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>